<commit_message>
Fixed inch conversion to mm
</commit_message>
<xml_diff>
--- a/data/Logan_Projection.xlsx
+++ b/data/Logan_Projection.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b6cb6b6143dae0d7/Documents/R/browser/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83D30190-8F6D-4290-84AB-67B2B850AE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{83D30190-8F6D-4290-84AB-67B2B850AE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C81E8EA7-78EF-45DD-9C74-AED4A1BCB140}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cache_County-monthly-proj_mod-t" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18">
     <font>
       <sz val="11"/>
@@ -907,11 +907,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -964,31 +964,31 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2025</v>
+        <v>2075</v>
       </c>
       <c r="C2">
-        <v>30.2</v>
+        <v>32.9</v>
       </c>
       <c r="D2">
-        <v>21.4</v>
+        <v>23.7</v>
       </c>
       <c r="E2">
-        <v>38.6</v>
+        <v>43.3</v>
       </c>
       <c r="F2">
-        <v>3.51</v>
+        <v>3.74</v>
       </c>
       <c r="G2">
-        <v>30.6</v>
+        <v>36</v>
       </c>
       <c r="H2">
-        <v>21.6</v>
+        <v>25.8</v>
       </c>
       <c r="I2">
-        <v>39.700000000000003</v>
+        <v>45.5</v>
       </c>
       <c r="J2">
-        <v>3.53</v>
+        <v>3.93</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -996,31 +996,31 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2025</v>
+        <v>2075</v>
       </c>
       <c r="C3">
-        <v>35.1</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="D3">
-        <v>24.4</v>
+        <v>28.1</v>
       </c>
       <c r="E3">
-        <v>45.8</v>
+        <v>50.9</v>
       </c>
       <c r="F3">
-        <v>2.91</v>
+        <v>3.03</v>
       </c>
       <c r="G3">
-        <v>35.5</v>
+        <v>42</v>
       </c>
       <c r="H3">
-        <v>25.8</v>
+        <v>30.7</v>
       </c>
       <c r="I3">
-        <v>46.7</v>
+        <v>54.7</v>
       </c>
       <c r="J3">
-        <v>2.9</v>
+        <v>3.26</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1028,31 +1028,31 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>2025</v>
+        <v>2075</v>
       </c>
       <c r="C4">
-        <v>45.6</v>
+        <v>49</v>
       </c>
       <c r="D4">
-        <v>35.799999999999997</v>
+        <v>38.4</v>
       </c>
       <c r="E4">
-        <v>57.2</v>
+        <v>64.3</v>
       </c>
       <c r="F4">
-        <v>2.69</v>
+        <v>2.89</v>
       </c>
       <c r="G4">
-        <v>45.7</v>
+        <v>51.6</v>
       </c>
       <c r="H4">
-        <v>35.799999999999997</v>
+        <v>40.6</v>
       </c>
       <c r="I4">
-        <v>58.3</v>
+        <v>65.8</v>
       </c>
       <c r="J4">
-        <v>2.76</v>
+        <v>3.21</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1060,31 +1060,31 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>2025</v>
+        <v>2075</v>
       </c>
       <c r="C5">
-        <v>55.7</v>
+        <v>58.3</v>
       </c>
       <c r="D5">
-        <v>45.8</v>
+        <v>47.6</v>
       </c>
       <c r="E5">
-        <v>67.099999999999994</v>
+        <v>71.5</v>
       </c>
       <c r="F5">
-        <v>2.85</v>
+        <v>3.07</v>
       </c>
       <c r="G5">
-        <v>55.4</v>
+        <v>60.7</v>
       </c>
       <c r="H5">
-        <v>45.5</v>
+        <v>50.2</v>
       </c>
       <c r="I5">
-        <v>66.599999999999994</v>
+        <v>73.5</v>
       </c>
       <c r="J5">
-        <v>2.98</v>
+        <v>3.11</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1092,31 +1092,31 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>2025</v>
+        <v>2075</v>
       </c>
       <c r="C6">
-        <v>66.400000000000006</v>
+        <v>69.400000000000006</v>
       </c>
       <c r="D6">
-        <v>57.6</v>
+        <v>59.7</v>
       </c>
       <c r="E6">
-        <v>75.400000000000006</v>
+        <v>78.400000000000006</v>
       </c>
       <c r="F6">
-        <v>2.58</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="G6">
-        <v>66.5</v>
+        <v>72.099999999999994</v>
       </c>
       <c r="H6">
-        <v>57.8</v>
+        <v>62.5</v>
       </c>
       <c r="I6">
-        <v>75.599999999999994</v>
+        <v>81.8</v>
       </c>
       <c r="J6">
-        <v>2.5499999999999998</v>
+        <v>2.38</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1124,31 +1124,31 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>2025</v>
+        <v>2075</v>
       </c>
       <c r="C7">
-        <v>75.900000000000006</v>
+        <v>79.2</v>
       </c>
       <c r="D7">
-        <v>67.2</v>
+        <v>70.099999999999994</v>
       </c>
       <c r="E7">
-        <v>84.3</v>
+        <v>87.9</v>
       </c>
       <c r="F7">
-        <v>1.5</v>
+        <v>1.46</v>
       </c>
       <c r="G7">
-        <v>76.2</v>
+        <v>82.7</v>
       </c>
       <c r="H7">
-        <v>67.900000000000006</v>
+        <v>72.7</v>
       </c>
       <c r="I7">
-        <v>84.4</v>
+        <v>92.7</v>
       </c>
       <c r="J7">
-        <v>1.52</v>
+        <v>1.31</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1156,31 +1156,31 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>2025</v>
+        <v>2075</v>
       </c>
       <c r="C8">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D8">
-        <v>79.5</v>
+        <v>81.599999999999994</v>
       </c>
       <c r="E8">
-        <v>90.9</v>
+        <v>95.3</v>
       </c>
       <c r="F8">
-        <v>0.77</v>
+        <v>0.83</v>
       </c>
       <c r="G8">
-        <v>85.9</v>
+        <v>92.9</v>
       </c>
       <c r="H8">
-        <v>79.900000000000006</v>
+        <v>85.5</v>
       </c>
       <c r="I8">
-        <v>91.2</v>
+        <v>100.6</v>
       </c>
       <c r="J8">
-        <v>0.82</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1188,31 +1188,31 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>2025</v>
+        <v>2075</v>
       </c>
       <c r="C9">
-        <v>84.2</v>
+        <v>87.6</v>
       </c>
       <c r="D9">
-        <v>78.8</v>
+        <v>81.099999999999994</v>
       </c>
       <c r="E9">
-        <v>89.5</v>
+        <v>95</v>
       </c>
       <c r="F9">
-        <v>1.1100000000000001</v>
+        <v>1.17</v>
       </c>
       <c r="G9">
-        <v>84.3</v>
+        <v>91.5</v>
       </c>
       <c r="H9">
-        <v>79.099999999999994</v>
+        <v>84.8</v>
       </c>
       <c r="I9">
-        <v>89.1</v>
+        <v>100.7</v>
       </c>
       <c r="J9">
-        <v>1.1000000000000001</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1220,31 +1220,31 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>2025</v>
+        <v>2075</v>
       </c>
       <c r="C10">
-        <v>74.099999999999994</v>
+        <v>77.400000000000006</v>
       </c>
       <c r="D10">
-        <v>67.099999999999994</v>
+        <v>69.5</v>
       </c>
       <c r="E10">
-        <v>80.8</v>
+        <v>84.9</v>
       </c>
       <c r="F10">
-        <v>1.53</v>
+        <v>1.6</v>
       </c>
       <c r="G10">
-        <v>74.2</v>
+        <v>80.900000000000006</v>
       </c>
       <c r="H10">
-        <v>67.3</v>
+        <v>73.400000000000006</v>
       </c>
       <c r="I10">
-        <v>81.099999999999994</v>
+        <v>89.5</v>
       </c>
       <c r="J10">
-        <v>1.6</v>
+        <v>1.71</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1252,31 +1252,31 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>2025</v>
+        <v>2075</v>
       </c>
       <c r="C11">
-        <v>60.9</v>
+        <v>63.7</v>
       </c>
       <c r="D11">
-        <v>53.1</v>
+        <v>55.4</v>
       </c>
       <c r="E11">
-        <v>69.099999999999994</v>
+        <v>72.599999999999994</v>
       </c>
       <c r="F11">
-        <v>1.89</v>
+        <v>1.92</v>
       </c>
       <c r="G11">
-        <v>61</v>
+        <v>67.3</v>
       </c>
       <c r="H11">
-        <v>52.3</v>
+        <v>58.7</v>
       </c>
       <c r="I11">
-        <v>69.099999999999994</v>
+        <v>76.400000000000006</v>
       </c>
       <c r="J11">
-        <v>1.98</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1284,31 +1284,31 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>2025</v>
+        <v>2075</v>
       </c>
       <c r="C12">
-        <v>43.2</v>
+        <v>45.9</v>
       </c>
       <c r="D12">
-        <v>35.200000000000003</v>
+        <v>36.5</v>
       </c>
       <c r="E12">
-        <v>52.5</v>
+        <v>54.3</v>
       </c>
       <c r="F12">
-        <v>3.06</v>
+        <v>2.93</v>
       </c>
       <c r="G12">
-        <v>43.4</v>
+        <v>48.3</v>
       </c>
       <c r="H12">
-        <v>34.700000000000003</v>
+        <v>39.299999999999997</v>
       </c>
       <c r="I12">
-        <v>52.3</v>
+        <v>57.3</v>
       </c>
       <c r="J12">
-        <v>2.86</v>
+        <v>2.87</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1316,798 +1316,30 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>2025</v>
+        <v>2075</v>
       </c>
       <c r="C13">
-        <v>31.1</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="D13">
-        <v>22.6</v>
+        <v>24.6</v>
       </c>
       <c r="E13">
-        <v>39.299999999999997</v>
+        <v>43.2</v>
       </c>
       <c r="F13">
-        <v>3.02</v>
+        <v>3</v>
       </c>
       <c r="G13">
-        <v>31.7</v>
+        <v>36.6</v>
       </c>
       <c r="H13">
-        <v>22.6</v>
+        <v>27.5</v>
       </c>
       <c r="I13">
-        <v>39.799999999999997</v>
+        <v>45.7</v>
       </c>
       <c r="J13">
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14">
-        <v>2050</v>
-      </c>
-      <c r="C14">
-        <v>31.8</v>
-      </c>
-      <c r="D14">
-        <v>22.7</v>
-      </c>
-      <c r="E14">
-        <v>42.4</v>
-      </c>
-      <c r="F14">
-        <v>3.56</v>
-      </c>
-      <c r="G14">
-        <v>32.9</v>
-      </c>
-      <c r="H14">
-        <v>23.3</v>
-      </c>
-      <c r="I14">
-        <v>43.2</v>
-      </c>
-      <c r="J14">
-        <v>3.75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15">
-        <v>2050</v>
-      </c>
-      <c r="C15">
-        <v>37.4</v>
-      </c>
-      <c r="D15">
-        <v>26.8</v>
-      </c>
-      <c r="E15">
-        <v>50.1</v>
-      </c>
-      <c r="F15">
-        <v>2.86</v>
-      </c>
-      <c r="G15">
-        <v>38.299999999999997</v>
-      </c>
-      <c r="H15">
-        <v>27.8</v>
-      </c>
-      <c r="I15">
-        <v>51.1</v>
-      </c>
-      <c r="J15">
-        <v>3.06</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16">
-        <v>3</v>
-      </c>
-      <c r="B16">
-        <v>2050</v>
-      </c>
-      <c r="C16">
-        <v>47.8</v>
-      </c>
-      <c r="D16">
-        <v>37.9</v>
-      </c>
-      <c r="E16">
-        <v>61.9</v>
-      </c>
-      <c r="F16">
-        <v>2.81</v>
-      </c>
-      <c r="G16">
-        <v>48.3</v>
-      </c>
-      <c r="H16">
-        <v>38.1</v>
-      </c>
-      <c r="I16">
-        <v>62.6</v>
-      </c>
-      <c r="J16">
-        <v>3.05</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17">
-        <v>4</v>
-      </c>
-      <c r="B17">
-        <v>2050</v>
-      </c>
-      <c r="C17">
-        <v>57.4</v>
-      </c>
-      <c r="D17">
-        <v>47</v>
-      </c>
-      <c r="E17">
-        <v>70.099999999999994</v>
-      </c>
-      <c r="F17">
-        <v>2.99</v>
-      </c>
-      <c r="G17">
-        <v>58.2</v>
-      </c>
-      <c r="H17">
-        <v>46.6</v>
-      </c>
-      <c r="I17">
-        <v>71</v>
-      </c>
-      <c r="J17">
-        <v>2.97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18">
-        <v>5</v>
-      </c>
-      <c r="B18">
-        <v>2050</v>
-      </c>
-      <c r="C18">
-        <v>68.2</v>
-      </c>
-      <c r="D18">
-        <v>59.1</v>
-      </c>
-      <c r="E18">
-        <v>76.900000000000006</v>
-      </c>
-      <c r="F18">
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="G18">
-        <v>69.3</v>
-      </c>
-      <c r="H18">
-        <v>59.8</v>
-      </c>
-      <c r="I18">
-        <v>78.7</v>
-      </c>
-      <c r="J18">
-        <v>2.42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19">
-        <v>6</v>
-      </c>
-      <c r="B19">
-        <v>2050</v>
-      </c>
-      <c r="C19">
-        <v>77.8</v>
-      </c>
-      <c r="D19">
-        <v>68.7</v>
-      </c>
-      <c r="E19">
-        <v>86</v>
-      </c>
-      <c r="F19">
-        <v>1.46</v>
-      </c>
-      <c r="G19">
-        <v>79.3</v>
-      </c>
-      <c r="H19">
-        <v>69.599999999999994</v>
-      </c>
-      <c r="I19">
-        <v>88</v>
-      </c>
-      <c r="J19">
-        <v>1.39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20">
-        <v>7</v>
-      </c>
-      <c r="B20">
-        <v>2050</v>
-      </c>
-      <c r="C20">
-        <v>87.8</v>
-      </c>
-      <c r="D20">
-        <v>81</v>
-      </c>
-      <c r="E20">
-        <v>93.6</v>
-      </c>
-      <c r="F20">
-        <v>0.83</v>
-      </c>
-      <c r="G20">
-        <v>89.1</v>
-      </c>
-      <c r="H20">
-        <v>82.1</v>
-      </c>
-      <c r="I20">
-        <v>95.5</v>
-      </c>
-      <c r="J20">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21">
-        <v>8</v>
-      </c>
-      <c r="B21">
-        <v>2050</v>
-      </c>
-      <c r="C21">
-        <v>86.2</v>
-      </c>
-      <c r="D21">
-        <v>79.8</v>
-      </c>
-      <c r="E21">
-        <v>92</v>
-      </c>
-      <c r="F21">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="G21">
-        <v>87.6</v>
-      </c>
-      <c r="H21">
-        <v>81.2</v>
-      </c>
-      <c r="I21">
-        <v>94.1</v>
-      </c>
-      <c r="J21">
-        <v>1.19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22">
-        <v>9</v>
-      </c>
-      <c r="B22">
-        <v>2050</v>
-      </c>
-      <c r="C22">
-        <v>75.900000000000006</v>
-      </c>
-      <c r="D22">
-        <v>68.5</v>
-      </c>
-      <c r="E22">
-        <v>83.1</v>
-      </c>
-      <c r="F22">
-        <v>1.63</v>
-      </c>
-      <c r="G22">
-        <v>77.2</v>
-      </c>
-      <c r="H22">
-        <v>69.3</v>
-      </c>
-      <c r="I22">
-        <v>84.7</v>
-      </c>
-      <c r="J22">
-        <v>1.53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23">
-        <v>10</v>
-      </c>
-      <c r="B23">
-        <v>2050</v>
-      </c>
-      <c r="C23">
-        <v>62.4</v>
-      </c>
-      <c r="D23">
-        <v>54</v>
-      </c>
-      <c r="E23">
-        <v>70.900000000000006</v>
-      </c>
-      <c r="F23">
-        <v>1.96</v>
-      </c>
-      <c r="G23">
-        <v>64</v>
-      </c>
-      <c r="H23">
-        <v>55.7</v>
-      </c>
-      <c r="I23">
-        <v>71.8</v>
-      </c>
-      <c r="J23">
-        <v>1.97</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24">
-        <v>11</v>
-      </c>
-      <c r="B24">
-        <v>2050</v>
-      </c>
-      <c r="C24">
-        <v>44.7</v>
-      </c>
-      <c r="D24">
-        <v>35.6</v>
-      </c>
-      <c r="E24">
-        <v>53.8</v>
-      </c>
-      <c r="F24">
-        <v>2.88</v>
-      </c>
-      <c r="G24">
-        <v>45.7</v>
-      </c>
-      <c r="H24">
-        <v>36.799999999999997</v>
-      </c>
-      <c r="I24">
-        <v>54.5</v>
-      </c>
-      <c r="J24">
-        <v>2.95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25">
-        <v>12</v>
-      </c>
-      <c r="B25">
-        <v>2050</v>
-      </c>
-      <c r="C25">
-        <v>32.700000000000003</v>
-      </c>
-      <c r="D25">
-        <v>24.3</v>
-      </c>
-      <c r="E25">
-        <v>41.6</v>
-      </c>
-      <c r="F25">
-        <v>2.97</v>
-      </c>
-      <c r="G25">
-        <v>34.1</v>
-      </c>
-      <c r="H25">
-        <v>25.1</v>
-      </c>
-      <c r="I25">
-        <v>42.7</v>
-      </c>
-      <c r="J25">
-        <v>3.15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="B26">
-        <v>2075</v>
-      </c>
-      <c r="C26">
-        <v>32.9</v>
-      </c>
-      <c r="D26">
-        <v>23.7</v>
-      </c>
-      <c r="E26">
-        <v>43.3</v>
-      </c>
-      <c r="F26">
-        <v>3.74</v>
-      </c>
-      <c r="G26">
-        <v>36</v>
-      </c>
-      <c r="H26">
-        <v>25.8</v>
-      </c>
-      <c r="I26">
-        <v>45.5</v>
-      </c>
-      <c r="J26">
-        <v>3.93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27">
-        <v>2</v>
-      </c>
-      <c r="B27">
-        <v>2075</v>
-      </c>
-      <c r="C27">
-        <v>38.799999999999997</v>
-      </c>
-      <c r="D27">
-        <v>28.1</v>
-      </c>
-      <c r="E27">
-        <v>50.9</v>
-      </c>
-      <c r="F27">
-        <v>3.03</v>
-      </c>
-      <c r="G27">
-        <v>42</v>
-      </c>
-      <c r="H27">
-        <v>30.7</v>
-      </c>
-      <c r="I27">
-        <v>54.7</v>
-      </c>
-      <c r="J27">
-        <v>3.26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28">
-        <v>3</v>
-      </c>
-      <c r="B28">
-        <v>2075</v>
-      </c>
-      <c r="C28">
-        <v>49</v>
-      </c>
-      <c r="D28">
-        <v>38.4</v>
-      </c>
-      <c r="E28">
-        <v>64.3</v>
-      </c>
-      <c r="F28">
-        <v>2.89</v>
-      </c>
-      <c r="G28">
-        <v>51.6</v>
-      </c>
-      <c r="H28">
-        <v>40.6</v>
-      </c>
-      <c r="I28">
-        <v>65.8</v>
-      </c>
-      <c r="J28">
-        <v>3.21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29">
-        <v>4</v>
-      </c>
-      <c r="B29">
-        <v>2075</v>
-      </c>
-      <c r="C29">
-        <v>58.3</v>
-      </c>
-      <c r="D29">
-        <v>47.6</v>
-      </c>
-      <c r="E29">
-        <v>71.5</v>
-      </c>
-      <c r="F29">
-        <v>3.07</v>
-      </c>
-      <c r="G29">
-        <v>60.7</v>
-      </c>
-      <c r="H29">
-        <v>50.2</v>
-      </c>
-      <c r="I29">
-        <v>73.5</v>
-      </c>
-      <c r="J29">
-        <v>3.11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30">
-        <v>5</v>
-      </c>
-      <c r="B30">
-        <v>2075</v>
-      </c>
-      <c r="C30">
-        <v>69.400000000000006</v>
-      </c>
-      <c r="D30">
-        <v>59.7</v>
-      </c>
-      <c r="E30">
-        <v>78.400000000000006</v>
-      </c>
-      <c r="F30">
-        <v>2.4700000000000002</v>
-      </c>
-      <c r="G30">
-        <v>72.099999999999994</v>
-      </c>
-      <c r="H30">
-        <v>62.5</v>
-      </c>
-      <c r="I30">
-        <v>81.8</v>
-      </c>
-      <c r="J30">
-        <v>2.38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31">
-        <v>6</v>
-      </c>
-      <c r="B31">
-        <v>2075</v>
-      </c>
-      <c r="C31">
-        <v>79.2</v>
-      </c>
-      <c r="D31">
-        <v>70.099999999999994</v>
-      </c>
-      <c r="E31">
-        <v>87.9</v>
-      </c>
-      <c r="F31">
-        <v>1.46</v>
-      </c>
-      <c r="G31">
-        <v>82.7</v>
-      </c>
-      <c r="H31">
-        <v>72.7</v>
-      </c>
-      <c r="I31">
-        <v>92.7</v>
-      </c>
-      <c r="J31">
-        <v>1.31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32">
-        <v>7</v>
-      </c>
-      <c r="B32">
-        <v>2075</v>
-      </c>
-      <c r="C32">
-        <v>89</v>
-      </c>
-      <c r="D32">
-        <v>81.599999999999994</v>
-      </c>
-      <c r="E32">
-        <v>95.3</v>
-      </c>
-      <c r="F32">
-        <v>0.83</v>
-      </c>
-      <c r="G32">
-        <v>92.9</v>
-      </c>
-      <c r="H32">
-        <v>85.5</v>
-      </c>
-      <c r="I32">
-        <v>100.6</v>
-      </c>
-      <c r="J32">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33">
-        <v>8</v>
-      </c>
-      <c r="B33">
-        <v>2075</v>
-      </c>
-      <c r="C33">
-        <v>87.6</v>
-      </c>
-      <c r="D33">
-        <v>81.099999999999994</v>
-      </c>
-      <c r="E33">
-        <v>95</v>
-      </c>
-      <c r="F33">
-        <v>1.17</v>
-      </c>
-      <c r="G33">
-        <v>91.5</v>
-      </c>
-      <c r="H33">
-        <v>84.8</v>
-      </c>
-      <c r="I33">
-        <v>100.7</v>
-      </c>
-      <c r="J33">
-        <v>1.29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34">
-        <v>9</v>
-      </c>
-      <c r="B34">
-        <v>2075</v>
-      </c>
-      <c r="C34">
-        <v>77.400000000000006</v>
-      </c>
-      <c r="D34">
-        <v>69.5</v>
-      </c>
-      <c r="E34">
-        <v>84.9</v>
-      </c>
-      <c r="F34">
-        <v>1.6</v>
-      </c>
-      <c r="G34">
-        <v>80.900000000000006</v>
-      </c>
-      <c r="H34">
-        <v>73.400000000000006</v>
-      </c>
-      <c r="I34">
-        <v>89.5</v>
-      </c>
-      <c r="J34">
-        <v>1.71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35">
-        <v>10</v>
-      </c>
-      <c r="B35">
-        <v>2075</v>
-      </c>
-      <c r="C35">
-        <v>63.7</v>
-      </c>
-      <c r="D35">
-        <v>55.4</v>
-      </c>
-      <c r="E35">
-        <v>72.599999999999994</v>
-      </c>
-      <c r="F35">
-        <v>1.92</v>
-      </c>
-      <c r="G35">
-        <v>67.3</v>
-      </c>
-      <c r="H35">
-        <v>58.7</v>
-      </c>
-      <c r="I35">
-        <v>76.400000000000006</v>
-      </c>
-      <c r="J35">
-        <v>1.83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36">
-        <v>11</v>
-      </c>
-      <c r="B36">
-        <v>2075</v>
-      </c>
-      <c r="C36">
-        <v>45.9</v>
-      </c>
-      <c r="D36">
-        <v>36.5</v>
-      </c>
-      <c r="E36">
-        <v>54.3</v>
-      </c>
-      <c r="F36">
-        <v>2.93</v>
-      </c>
-      <c r="G36">
-        <v>48.3</v>
-      </c>
-      <c r="H36">
-        <v>39.299999999999997</v>
-      </c>
-      <c r="I36">
-        <v>57.3</v>
-      </c>
-      <c r="J36">
-        <v>2.87</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="A37">
-        <v>12</v>
-      </c>
-      <c r="B37">
-        <v>2075</v>
-      </c>
-      <c r="C37">
-        <v>33.700000000000003</v>
-      </c>
-      <c r="D37">
-        <v>24.6</v>
-      </c>
-      <c r="E37">
-        <v>43.2</v>
-      </c>
-      <c r="F37">
-        <v>3</v>
-      </c>
-      <c r="G37">
-        <v>36.6</v>
-      </c>
-      <c r="H37">
-        <v>27.5</v>
-      </c>
-      <c r="I37">
-        <v>45.7</v>
-      </c>
-      <c r="J37">
         <v>3.17</v>
       </c>
     </row>

</xml_diff>